<commit_message>
modification to low load base prime file
</commit_message>
<xml_diff>
--- a/logFile_20160601.xlsx
+++ b/logFile_20160601.xlsx
@@ -4382,8 +4382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:T1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4553,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H6" si="4">H5-0.057</f>
+        <f>H5-0.057</f>
         <v>0.7719999999999998</v>
       </c>
       <c r="J4">
@@ -4561,15 +4561,15 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K47" si="5">LN(F4)</f>
+        <f t="shared" ref="K4:K47" si="4">LN(F4)</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L47" si="6">LOG10(F4)</f>
+        <f t="shared" ref="L4:L47" si="5">LOG10(F4)</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M47" si="7">LOG(F4,6)</f>
+        <f t="shared" ref="M4:M47" si="6">LOG(F4,6)</f>
         <v>0</v>
       </c>
       <c r="N4" s="1">
@@ -4615,7 +4615,7 @@
         <v>2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H4:H6" si="7">H6-0.057</f>
         <v>0.82899999999999985</v>
       </c>
       <c r="J5">
@@ -4623,15 +4623,15 @@
         <v>1</v>
       </c>
       <c r="K5">
+        <f t="shared" si="4"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="5"/>
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="L5">
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="6"/>
-        <v>0.3010299956639812</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="7"/>
         <v>0.38685280723454157</v>
       </c>
       <c r="N5" s="1">
@@ -4677,7 +4677,7 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.8859999999999999</v>
       </c>
       <c r="J6">
@@ -4685,15 +4685,15 @@
         <v>0</v>
       </c>
       <c r="K6">
+        <f t="shared" si="4"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="5"/>
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="L6">
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="6"/>
-        <v>0.3010299956639812</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="7"/>
         <v>0.38685280723454157</v>
       </c>
       <c r="N6" s="1">
@@ -4747,15 +4747,15 @@
         <v>0</v>
       </c>
       <c r="K7">
+        <f t="shared" si="4"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="5"/>
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="L7">
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="6"/>
-        <v>0.3010299956639812</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="7"/>
         <v>0.38685280723454157</v>
       </c>
       <c r="N7" s="1">
@@ -4813,15 +4813,15 @@
         <v>2</v>
       </c>
       <c r="K8">
+        <f t="shared" si="4"/>
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="5"/>
-        <v>1.3862943611198906</v>
-      </c>
-      <c r="L8">
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="6"/>
-        <v>0.6020599913279624</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="7"/>
         <v>0.77370561446908315</v>
       </c>
       <c r="N8" s="1">
@@ -4879,15 +4879,15 @@
         <v>0</v>
       </c>
       <c r="K9">
+        <f t="shared" si="4"/>
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="5"/>
-        <v>1.3862943611198906</v>
-      </c>
-      <c r="L9">
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="6"/>
-        <v>0.6020599913279624</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="7"/>
         <v>0.77370561446908315</v>
       </c>
       <c r="N9" s="1">
@@ -4945,15 +4945,15 @@
         <v>2</v>
       </c>
       <c r="K10">
+        <f t="shared" si="4"/>
+        <v>1.791759469228055</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="5"/>
-        <v>1.791759469228055</v>
-      </c>
-      <c r="L10">
+        <v>0.77815125038364363</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="6"/>
-        <v>0.77815125038364363</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N10" s="1">
@@ -5011,15 +5011,15 @@
         <v>2</v>
       </c>
       <c r="K11">
+        <f t="shared" si="4"/>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="5"/>
-        <v>2.0794415416798357</v>
-      </c>
-      <c r="L11">
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="6"/>
-        <v>0.90308998699194354</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="7"/>
         <v>1.1605584217036247</v>
       </c>
       <c r="N11" s="1">
@@ -5077,15 +5077,15 @@
         <v>4</v>
       </c>
       <c r="K12">
+        <f t="shared" si="4"/>
+        <v>2.4849066497880004</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="5"/>
-        <v>2.4849066497880004</v>
-      </c>
-      <c r="L12">
+        <v>1.0791812460476249</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="6"/>
-        <v>1.0791812460476249</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="7"/>
         <v>1.3868528072345416</v>
       </c>
       <c r="N12" s="1">
@@ -5143,15 +5143,15 @@
         <v>1</v>
       </c>
       <c r="K13">
+        <f t="shared" si="4"/>
+        <v>2.5649493574615367</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="5"/>
-        <v>2.5649493574615367</v>
-      </c>
-      <c r="L13">
+        <v>1.1139433523068367</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="6"/>
-        <v>1.1139433523068367</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="7"/>
         <v>1.4315254929650774</v>
       </c>
       <c r="N13" s="1">
@@ -5209,15 +5209,15 @@
         <v>6</v>
       </c>
       <c r="K14">
+        <f t="shared" si="4"/>
+        <v>2.9444389791664403</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="5"/>
-        <v>2.9444389791664403</v>
-      </c>
-      <c r="L14">
+        <v>1.2787536009528289</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="6"/>
-        <v>1.2787536009528289</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="7"/>
         <v>1.643322683504497</v>
       </c>
       <c r="N14" s="1">
@@ -5275,15 +5275,15 @@
         <v>5</v>
       </c>
       <c r="K15">
+        <f t="shared" si="4"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="5"/>
-        <v>3.1780538303479458</v>
-      </c>
-      <c r="L15">
+        <v>1.3802112417116059</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="6"/>
-        <v>1.3802112417116059</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="7"/>
         <v>1.7737056144690833</v>
       </c>
       <c r="N15" s="1">
@@ -5341,15 +5341,15 @@
         <v>12</v>
       </c>
       <c r="K16">
+        <f t="shared" si="4"/>
+        <v>3.5835189384561099</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="5"/>
-        <v>3.5835189384561099</v>
-      </c>
-      <c r="L16">
+        <v>1.5563025007672873</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="6"/>
-        <v>1.5563025007672873</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="N16" s="1">
@@ -5407,15 +5407,15 @@
         <v>12</v>
       </c>
       <c r="K17">
+        <f t="shared" si="4"/>
+        <v>3.8712010109078911</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="5"/>
-        <v>3.8712010109078911</v>
-      </c>
-      <c r="L17">
+        <v>1.6812412373755872</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="6"/>
-        <v>1.6812412373755872</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="7"/>
         <v>2.1605584217036249</v>
       </c>
       <c r="N17" s="1">
@@ -5473,15 +5473,15 @@
         <v>13</v>
       </c>
       <c r="K18">
+        <f t="shared" si="4"/>
+        <v>4.1108738641733114</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="5"/>
-        <v>4.1108738641733114</v>
-      </c>
-      <c r="L18">
+        <v>1.7853298350107671</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="6"/>
-        <v>1.7853298350107671</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="7"/>
         <v>2.2943223880069139</v>
       </c>
       <c r="N18" s="1">
@@ -5539,15 +5539,15 @@
         <v>22</v>
       </c>
       <c r="K19">
+        <f t="shared" si="4"/>
+        <v>4.4188406077965983</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="5"/>
-        <v>4.4188406077965983</v>
-      </c>
-      <c r="L19">
+        <v>1.919078092376074</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="6"/>
-        <v>1.919078092376074</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="7"/>
         <v>2.4662019002474538</v>
       </c>
       <c r="N19" s="1">
@@ -5605,15 +5605,15 @@
         <v>33</v>
       </c>
       <c r="K20">
+        <f t="shared" si="4"/>
+        <v>4.7535901911063645</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="5"/>
-        <v>4.7535901911063645</v>
-      </c>
-      <c r="L20">
+        <v>2.0644579892269186</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="6"/>
-        <v>2.0644579892269186</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="7"/>
         <v>2.6530291999262365</v>
       </c>
       <c r="N20" s="1">
@@ -5671,15 +5671,15 @@
         <v>39</v>
       </c>
       <c r="K21">
+        <f t="shared" si="4"/>
+        <v>5.0434251169192468</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="5"/>
-        <v>5.0434251169192468</v>
-      </c>
-      <c r="L21">
+        <v>2.1903316981702914</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="6"/>
-        <v>2.1903316981702914</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="7"/>
         <v>2.8147891519680983</v>
       </c>
       <c r="N21" s="1">
@@ -5737,15 +5737,15 @@
         <v>58</v>
       </c>
       <c r="K22">
+        <f t="shared" si="4"/>
+        <v>5.3612921657094255</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="5"/>
-        <v>5.3612921657094255</v>
-      </c>
-      <c r="L22">
+        <v>2.3283796034387376</v>
+      </c>
+      <c r="M22">
         <f t="shared" si="6"/>
-        <v>2.3283796034387376</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="7"/>
         <v>2.9921941297283809</v>
       </c>
       <c r="N22" s="1">
@@ -5803,15 +5803,15 @@
         <v>73</v>
       </c>
       <c r="K23">
+        <f t="shared" si="4"/>
+        <v>5.6559918108198524</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="5"/>
-        <v>5.6559918108198524</v>
-      </c>
-      <c r="L23">
+        <v>2.4563660331290431</v>
+      </c>
+      <c r="M23">
         <f t="shared" si="6"/>
-        <v>2.4563660331290431</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="7"/>
         <v>3.1566691333053916</v>
       </c>
       <c r="N23" s="1">
@@ -5869,15 +5869,15 @@
         <v>110</v>
       </c>
       <c r="K24">
+        <f t="shared" si="4"/>
+        <v>5.9814142112544806</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="5"/>
-        <v>5.9814142112544806</v>
-      </c>
-      <c r="L24">
+        <v>2.5976951859255122</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="6"/>
-        <v>2.5976951859255122</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="7"/>
         <v>3.3382908331057726</v>
       </c>
       <c r="N24" s="1">
@@ -5935,15 +5935,15 @@
         <v>136</v>
       </c>
       <c r="K25">
+        <f t="shared" si="4"/>
+        <v>6.2766434893416445</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="5"/>
-        <v>6.2766434893416445</v>
-      </c>
-      <c r="L25">
+        <v>2.7259116322950483</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="6"/>
-        <v>2.7259116322950483</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="7"/>
         <v>3.5030614304752721</v>
       </c>
       <c r="N25" s="1">
@@ -6001,15 +6001,15 @@
         <v>207</v>
       </c>
       <c r="K26">
+        <f t="shared" si="4"/>
+        <v>6.6052979209482015</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="5"/>
-        <v>6.6052979209482015</v>
-      </c>
-      <c r="L26">
+        <v>2.8686444383948255</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="6"/>
-        <v>2.8686444383948255</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="7"/>
         <v>3.6864869612180517</v>
       </c>
       <c r="N26" s="1">
@@ -6067,15 +6067,15 @@
         <v>254</v>
       </c>
       <c r="K27">
+        <f t="shared" si="4"/>
+        <v>6.9007306640451729</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="5"/>
-        <v>6.9007306640451729</v>
-      </c>
-      <c r="L27">
+        <v>2.996949248495381</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="6"/>
-        <v>2.996949248495381</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="7"/>
         <v>3.851371114571656</v>
       </c>
       <c r="N27" s="1">
@@ -6133,15 +6133,15 @@
         <v>391</v>
       </c>
       <c r="K28">
+        <f t="shared" si="4"/>
+        <v>7.2327331361776146</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="5"/>
-        <v>7.2327331361776146</v>
-      </c>
-      <c r="L28">
+        <v>3.1411360901207388</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="6"/>
-        <v>3.1411360901207388</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="7"/>
         <v>4.0366652223100559</v>
       </c>
       <c r="N28" s="1">
@@ -6199,15 +6199,15 @@
         <v>464</v>
       </c>
       <c r="K29">
+        <f t="shared" si="4"/>
+        <v>7.5218592522016294</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="5"/>
-        <v>7.5218592522016294</v>
-      </c>
-      <c r="L29">
+        <v>3.2667019668840878</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="6"/>
-        <v>3.2667019668840878</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="7"/>
         <v>4.1980295800765477</v>
       </c>
       <c r="N29" s="1">
@@ -6265,15 +6265,15 @@
         <v>768</v>
       </c>
       <c r="K30">
+        <f t="shared" si="4"/>
+        <v>7.8694017125770896</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="5"/>
-        <v>7.8694017125770896</v>
-      </c>
-      <c r="L30">
+        <v>3.4176377396522297</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="6"/>
-        <v>3.4176377396522297</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="7"/>
         <v>4.3919967203898578</v>
       </c>
       <c r="N30" s="1">
@@ -6331,15 +6331,15 @@
         <v>884</v>
       </c>
       <c r="K31">
+        <f t="shared" si="4"/>
+        <v>8.1605182474775049</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="5"/>
-        <v>8.1605182474775049</v>
-      </c>
-      <c r="L31">
+        <v>3.5440680443502757</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="6"/>
-        <v>3.5440680443502757</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="7"/>
         <v>4.5544719520825563</v>
       </c>
       <c r="N31" s="1">
@@ -6397,15 +6397,15 @@
         <v>1411</v>
       </c>
       <c r="K32">
+        <f t="shared" si="4"/>
+        <v>8.4992328660392449</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="5"/>
-        <v>8.4992328660392449</v>
-      </c>
-      <c r="L32">
+        <v>3.691169934131604</v>
+      </c>
+      <c r="M32">
         <f t="shared" si="6"/>
-        <v>3.691169934131604</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="7"/>
         <v>4.7435121800701161</v>
       </c>
       <c r="N32" s="1">
@@ -6463,15 +6463,15 @@
         <v>1697</v>
       </c>
       <c r="K33">
+        <f t="shared" si="4"/>
+        <v>8.7960363152008139</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="5"/>
-        <v>8.7960363152008139</v>
-      </c>
-      <c r="L33">
+        <v>3.8200700343123257</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="6"/>
-        <v>3.8200700343123257</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="7"/>
         <v>4.9091613390442506</v>
       </c>
       <c r="N33" s="1">
@@ -6529,15 +6529,15 @@
         <v>2683</v>
       </c>
       <c r="K34">
+        <f t="shared" si="4"/>
+        <v>9.1368014686413126</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="5"/>
-        <v>9.1368014686413126</v>
-      </c>
-      <c r="L34">
+        <v>3.9680624600764491</v>
+      </c>
+      <c r="M34">
         <f t="shared" si="6"/>
-        <v>3.9680624600764491</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="7"/>
         <v>5.0993459923377591</v>
       </c>
       <c r="N34" s="1">
@@ -6595,15 +6595,15 @@
         <v>3208</v>
       </c>
       <c r="K35">
+        <f t="shared" si="4"/>
+        <v>9.4334039200902211</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="5"/>
-        <v>9.4334039200902211</v>
-      </c>
-      <c r="L35">
+        <v>4.096875268059688</v>
+      </c>
+      <c r="M35">
         <f t="shared" si="6"/>
-        <v>4.096875268059688</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="7"/>
         <v>5.2648829723525452</v>
       </c>
       <c r="N35" s="1">
@@ -6661,15 +6661,15 @@
         <v>5162</v>
       </c>
       <c r="K36">
+        <f t="shared" si="4"/>
+        <v>9.7791140976963717</v>
+      </c>
+      <c r="L36">
         <f t="shared" si="5"/>
-        <v>9.7791140976963717</v>
-      </c>
-      <c r="L36">
+        <v>4.2470152905318317</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="6"/>
-        <v>4.2470152905318317</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="7"/>
         <v>5.4578274961814568</v>
       </c>
       <c r="N36" s="1">
@@ -6727,15 +6727,15 @@
         <v>6083</v>
       </c>
       <c r="K37">
+        <f t="shared" si="4"/>
+        <v>10.075085145967106</v>
+      </c>
+      <c r="L37">
         <f t="shared" si="5"/>
-        <v>10.075085145967106</v>
-      </c>
-      <c r="L37">
+        <v>4.3755538835989327</v>
+      </c>
+      <c r="M37">
         <f t="shared" si="6"/>
-        <v>4.3755538835989327</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="7"/>
         <v>5.6230120833728661</v>
       </c>
       <c r="N37" s="1">
@@ -6793,15 +6793,15 @@
         <v>9804</v>
       </c>
       <c r="K38">
+        <f t="shared" si="4"/>
+        <v>10.420732528104303</v>
+      </c>
+      <c r="L38">
         <f t="shared" si="5"/>
-        <v>10.420732528104303</v>
-      </c>
-      <c r="L38">
+        <v>4.5256666343454217</v>
+      </c>
+      <c r="M38">
         <f t="shared" si="6"/>
-        <v>4.5256666343454217</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="7"/>
         <v>5.8159215603832557</v>
       </c>
       <c r="N38" s="1">
@@ -6859,15 +6859,15 @@
         <v>11734</v>
       </c>
       <c r="K39">
+        <f t="shared" si="4"/>
+        <v>10.720664881512924</v>
+      </c>
+      <c r="L39">
         <f t="shared" si="5"/>
-        <v>10.720664881512924</v>
-      </c>
-      <c r="L39">
+        <v>4.655925600375042</v>
+      </c>
+      <c r="M39">
         <f t="shared" si="6"/>
-        <v>4.655925600375042</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="7"/>
         <v>5.9833169940671311</v>
       </c>
       <c r="N39" s="1">
@@ -6925,15 +6925,15 @@
         <v>18708</v>
       </c>
       <c r="K40">
+        <f t="shared" si="4"/>
+        <v>11.066482100133506</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="5"/>
-        <v>11.066482100133506</v>
-      </c>
-      <c r="L40">
+        <v>4.8061121101690913</v>
+      </c>
+      <c r="M40">
         <f t="shared" si="6"/>
-        <v>4.8061121101690913</v>
-      </c>
-      <c r="M40">
-        <f t="shared" si="7"/>
         <v>6.1763212586236733</v>
       </c>
       <c r="N40" s="1">
@@ -6991,15 +6991,15 @@
         <v>22383</v>
       </c>
       <c r="K41">
+        <f t="shared" si="4"/>
+        <v>11.366430405953848</v>
+      </c>
+      <c r="L41">
         <f t="shared" si="5"/>
-        <v>11.366430405953848</v>
-      </c>
-      <c r="L41">
+        <v>4.9363780042430943</v>
+      </c>
+      <c r="M41">
         <f t="shared" si="6"/>
-        <v>4.9363780042430943</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="7"/>
         <v>6.34372559551805</v>
       </c>
       <c r="N41" s="1">
@@ -7057,15 +7057,15 @@
         <v>35826</v>
       </c>
       <c r="K42">
+        <f t="shared" si="4"/>
+        <v>11.713406142380093</v>
+      </c>
+      <c r="L42">
         <f t="shared" si="5"/>
-        <v>11.713406142380093</v>
-      </c>
-      <c r="L42">
+        <v>5.0870676519273301</v>
+      </c>
+      <c r="M42">
         <f t="shared" si="6"/>
-        <v>5.0870676519273301</v>
-      </c>
-      <c r="M42">
-        <f t="shared" si="7"/>
         <v>6.5373764411729818</v>
       </c>
       <c r="N42" s="1">
@@ -7123,15 +7123,15 @@
         <v>43075</v>
       </c>
       <c r="K43">
+        <f t="shared" si="4"/>
+        <v>12.015359981661616</v>
+      </c>
+      <c r="L43">
         <f t="shared" si="5"/>
-        <v>12.015359981661616</v>
-      </c>
-      <c r="L43">
+        <v>5.2182045381167974</v>
+      </c>
+      <c r="M43">
         <f t="shared" si="6"/>
-        <v>5.2182045381167974</v>
-      </c>
-      <c r="M43">
-        <f t="shared" si="7"/>
         <v>6.7059000876039478</v>
       </c>
       <c r="N43" s="1">
@@ -7189,15 +7189,15 @@
         <v>68881</v>
       </c>
       <c r="K44">
+        <f t="shared" si="4"/>
+        <v>12.363738568216711</v>
+      </c>
+      <c r="L44">
         <f t="shared" si="5"/>
-        <v>12.363738568216711</v>
-      </c>
-      <c r="L44">
+        <v>5.3695034358709295</v>
+      </c>
+      <c r="M44">
         <f t="shared" si="6"/>
-        <v>5.3695034358709295</v>
-      </c>
-      <c r="M44">
-        <f t="shared" si="7"/>
         <v>6.9003338788232496</v>
       </c>
       <c r="N44" s="1">
@@ -7255,15 +7255,15 @@
         <v>82470</v>
       </c>
       <c r="K45">
+        <f t="shared" si="4"/>
+        <v>12.665473387303976</v>
+      </c>
+      <c r="L45">
         <f t="shared" si="5"/>
-        <v>12.665473387303976</v>
-      </c>
-      <c r="L45">
+        <v>5.5005452027986044</v>
+      </c>
+      <c r="M45">
         <f t="shared" si="6"/>
-        <v>5.5005452027986044</v>
-      </c>
-      <c r="M45">
-        <f t="shared" si="7"/>
         <v>7.0687352877563701</v>
       </c>
       <c r="N45" s="1">
@@ -7321,15 +7321,15 @@
         <v>132145</v>
       </c>
       <c r="K46">
+        <f t="shared" si="4"/>
+        <v>13.014265786036617</v>
+      </c>
+      <c r="L46">
         <f t="shared" si="5"/>
-        <v>13.014265786036617</v>
-      </c>
-      <c r="L46">
+        <v>5.6520238168979891</v>
+      </c>
+      <c r="M46">
         <f t="shared" si="6"/>
-        <v>5.6520238168979891</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="7"/>
         <v>7.2634000319493568</v>
       </c>
       <c r="N46" s="1">
@@ -7387,15 +7387,15 @@
         <v>159057</v>
       </c>
       <c r="K47">
+        <f t="shared" si="4"/>
+        <v>13.317645580985584</v>
+      </c>
+      <c r="L47">
         <f t="shared" si="5"/>
-        <v>13.317645580985584</v>
-      </c>
-      <c r="L47">
+        <v>5.7837799877652651</v>
+      </c>
+      <c r="M47">
         <f t="shared" si="6"/>
-        <v>5.7837799877652651</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="7"/>
         <v>7.4327195193913136</v>
       </c>
       <c r="N47" s="1">

</xml_diff>